<commit_message>
Update With New Issues
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmed\Documents\UiPath\RaryaJumiaSearchProduct\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E18B323B-4F57-4DEA-B4FC-267EF246FB08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BF16C4E-A0E0-4DD3-88EE-1F9F9B053156}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6000" yWindow="3090" windowWidth="18000" windowHeight="9810" xr2:uid="{C6AE6A82-7BAD-415A-B62A-6E1180E09E42}"/>
+    <workbookView xWindow="6000" yWindow="3090" windowWidth="18000" windowHeight="9810" xr2:uid="{7A8F9DF8-C676-4464-9FEA-608D890C8465}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Jumia" sheetId="3" r:id="rId1"/>
+    <sheet name="Raya" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="72">
   <si>
     <t>Name</t>
   </si>
@@ -42,43 +44,214 @@
     <t>Price</t>
   </si>
   <si>
-    <t>Devia Screen Protector Intelligent Screen Antibacterial for Samsung Galaxy Note 20 Ultra - Clear</t>
-  </si>
-  <si>
-    <t>Baseus Type-C Cable Fast Charging, 1 Meter, 3mAh, For Samsung Galaxy Note 20 Ultra - White</t>
-  </si>
-  <si>
-    <t>Ozo Skins Tropical Flamingo Pink For Samsung Galaxy Note 20 Ultra - SE163TFP</t>
-  </si>
-  <si>
-    <t>Ozo Skins ِAl-Ahly SC For Samsung Galaxy Note 20 Ultra - SE114ASC</t>
-  </si>
-  <si>
-    <t>Ozo Skins Black Pink Marble For Samsung Galaxy Note 20 Ultra - SE114ASC</t>
-  </si>
-  <si>
-    <t>Anank Glass 3D Screen Protector For Samsung Galaxy Note20 Ultra</t>
-  </si>
-  <si>
-    <t>Armor Screen Easy Full body for Samsung Galaxy Note 20 Ultra</t>
-  </si>
-  <si>
-    <t>Samsung Protective Cover For Samsung Galaxy Note 20 Ultra - Clear Black</t>
-  </si>
-  <si>
-    <t>Samsung Galaxy Note 20 Ultra Dual SIM, 256GB, 8GB RAM, 4G LTE, Black</t>
-  </si>
-  <si>
-    <t>Samsung Galaxy Note 20 Ultra Dual SIM, 256GB, 8GB RAM, 4G LTE , Mystic Black</t>
-  </si>
-  <si>
-    <t>Samsung Galaxy Note 20 Ultra Dual SIM, 256GB, 8GB RAM, 4G LTE, Mystic Black</t>
-  </si>
-  <si>
-    <t>Samsung Galaxy Note 20 Ultra Dual SIM, 256GB, 8GB RAM, 4G LTE, Mystic Bronze</t>
-  </si>
-  <si>
-    <t>Samsung Galaxy Note 20 Ultra Dual SIM, 256GB, 8GB RAM, 4G LTE, Mystic White</t>
+    <t>EGP 39</t>
+  </si>
+  <si>
+    <t>For Samsung Galaxy Note20 Ultra IMAK UC-2 Series Shockproof Full Coverage Soft TPU Case(Yellow)</t>
+  </si>
+  <si>
+    <t>For Samsung Galaxy Note20 Ultra IMAK UC-2 Series Shockproof Full Coverage Soft TPU Case(Red)</t>
+  </si>
+  <si>
+    <t>EGP 49</t>
+  </si>
+  <si>
+    <t>For Samsung Galaxy Note20 Ultra Luminous TPU Soft Protective Case(Owl)</t>
+  </si>
+  <si>
+    <t>For Samsung Galaxy Note20 Ultra Skin Hand Feeling Series Shockproof Frosted PC+ TPU Protective Case(Black)</t>
+  </si>
+  <si>
+    <t>For Samsung Galaxy Note20 Ultra Luminous TPU Soft Protective Case(Black Wind Chimes)</t>
+  </si>
+  <si>
+    <t>For Samsung Galaxy Note20 Ultra Luminous TPU Soft Protective Case(Rose Flower)</t>
+  </si>
+  <si>
+    <t>Case For Samsung Galaxy Note 20 Ultra Soft Silicone+Hard Fabric Deer Slim Casing</t>
+  </si>
+  <si>
+    <t>EGP 112</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy Note 20 Ultra Leather Case With Card Slot - Blue</t>
+  </si>
+  <si>
+    <t>EGP 118</t>
+  </si>
+  <si>
+    <t>For Samsung Galaxy Note20 Ultra Litchi Texture TPU Shockproof Case(Black)</t>
+  </si>
+  <si>
+    <t>EGP 79</t>
+  </si>
+  <si>
+    <t>Electric Waffles Maker Household Waffle Egg Cake Oven</t>
+  </si>
+  <si>
+    <t>Personal Portable Electric Oven Mini Mac Hot Logic Food Tote Picnic Camping</t>
+  </si>
+  <si>
+    <t>EGP 836</t>
+  </si>
+  <si>
+    <t>EGP 953</t>
+  </si>
+  <si>
+    <t>Armor PVC Back Cover For Nokia 6 - Transparent</t>
+  </si>
+  <si>
+    <t>EGP31.00</t>
+  </si>
+  <si>
+    <t>Armor Screen Nano Glass anti Fingerprint Matte for Nokia 1 Plus</t>
+  </si>
+  <si>
+    <t>EGP71.00</t>
+  </si>
+  <si>
+    <t>Armor Nano Glass anti broken Screen Protector for Nokia 6.1</t>
+  </si>
+  <si>
+    <t>EGP79.00</t>
+  </si>
+  <si>
+    <t>Armor Screen Nano Glass anti broken for Nokia C2</t>
+  </si>
+  <si>
+    <t>OZO Skins For Nokia 6.2, Vans Gary Stickers - SE142VGS</t>
+  </si>
+  <si>
+    <t>Ozo Skins For Nokia 6.2, Australian OAK Wood - SE154AOW</t>
+  </si>
+  <si>
+    <t>Ozo Skins For Nokia 6.2, Pharaonic Style - Se132ofs</t>
+  </si>
+  <si>
+    <t>Ozo Skins For Nokia 6.2, Black Pink Marble - SE130BPM</t>
+  </si>
+  <si>
+    <t>Armor Screen Protector With 4In1 Features Nano Material For Nokia 5</t>
+  </si>
+  <si>
+    <t>Armor Screen Protector With 4In1 Features Nano Material For Nokia C2</t>
+  </si>
+  <si>
+    <t>EGP89.00</t>
+  </si>
+  <si>
+    <t>Armor Nano Glass anti broken Screen Protector for Nokia 7.2</t>
+  </si>
+  <si>
+    <t>EGP95.00</t>
+  </si>
+  <si>
+    <t>Armor Screen Nano Glass anti Fingerprint Matte for Nokia 3</t>
+  </si>
+  <si>
+    <t>Armor Screen Nano Glass anti Fingerprint Matte for Nokia 5.3</t>
+  </si>
+  <si>
+    <t>Armor Screen Nano Anti Broken For Mobile Nokia 5.4</t>
+  </si>
+  <si>
+    <t>armor Screen Nano Glass anti broken for Nokia 5.3</t>
+  </si>
+  <si>
+    <t>EGP99.00</t>
+  </si>
+  <si>
+    <t>Armor Screen Protector With 4In1 Features Nano Material For Nokia 1.4</t>
+  </si>
+  <si>
+    <t>Armor Screen Protector With 4In1 Features Nano Material For Nokia 7.1</t>
+  </si>
+  <si>
+    <t>Armor Screen Protector With 4In1 Features Nano Material For Nokia 7.2</t>
+  </si>
+  <si>
+    <t>Armor Screen Nano Glass anti Fingerprint Matte for Nokia 6.2</t>
+  </si>
+  <si>
+    <t>EGP103.00</t>
+  </si>
+  <si>
+    <t>Armor Screen Nano Glass anti Fingerprint Matte for Nokia 7.2</t>
+  </si>
+  <si>
+    <t>Armor Screen Nano Glass anti Fingerprint Matte for Nokia 3.2</t>
+  </si>
+  <si>
+    <t>EGP111.00</t>
+  </si>
+  <si>
+    <t>Armor Screen Nano Glass anti Fingerprint Matte for Nokia 8</t>
+  </si>
+  <si>
+    <t>Armor Screen Nano Anti Blue Ray (Eye Guard) For Mobile Nokia 5.4</t>
+  </si>
+  <si>
+    <t>Armor Privacy Screen Protector For Nokia 5.4</t>
+  </si>
+  <si>
+    <t>EGP119.00</t>
+  </si>
+  <si>
+    <t>Armor Screen Protector With 4In1 Features Nano Material For Nokia 2.4</t>
+  </si>
+  <si>
+    <t>Armor Screen Protector With 4In1 Features Nano Material For Nokia 5.3</t>
+  </si>
+  <si>
+    <t>Armor Screen Protector With 4In1 Features Nano Material For Nokia 6</t>
+  </si>
+  <si>
+    <t>Armor Screen Protector With 4In1 Features Nano Material For Nokia 6.1</t>
+  </si>
+  <si>
+    <t>Armor Screen Protector With 5In1 Features Nano Material, Anti Fingerprint For Nokia 1.4</t>
+  </si>
+  <si>
+    <t>Nokia 6.1 Plus/Nokia X6 3 In 1 Hard PC Case - Red</t>
+  </si>
+  <si>
+    <t>EGP 15</t>
+  </si>
+  <si>
+    <t>Nokia 3.4 - 6.39-inch 64GB/4GB Dual SIM Mobile Phone - Charcoal Grey</t>
+  </si>
+  <si>
+    <t>EGP 2,022</t>
+  </si>
+  <si>
+    <t>Nokia 6300 4G – 2.4-inch 4G Dual SIM Mobile Phone - Charcoal</t>
+  </si>
+  <si>
+    <t>EGP 949</t>
+  </si>
+  <si>
+    <t>Nokia 3.2 - 6.26-inch 32GB/3GB Mobile Phone - Steel</t>
+  </si>
+  <si>
+    <t>EGP 1,849</t>
+  </si>
+  <si>
+    <t>Nokia 3.2 - 6.26-inch 32GB/3GB Mobile Phone - Black</t>
+  </si>
+  <si>
+    <t>Nokia 3.4 - 6.39-inch 64GB/4GB Dual SIM Mobile Phone - Fjord Blue</t>
+  </si>
+  <si>
+    <t>EGP 2,222</t>
+  </si>
+  <si>
+    <t>Nokia 225 - 2.4-inch Dual Sim 4G Mobile Phone - Sand</t>
+  </si>
+  <si>
+    <t>EGP 729</t>
+  </si>
+  <si>
+    <t>Nokia 3.4 - 6.39-inch 64GB/4GB Dual SIM Mobile Phone - Dusk Purple</t>
   </si>
 </sst>
 </file>
@@ -94,12 +267,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -114,8 +299,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -429,126 +616,466 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C06DAA54-077A-4AE2-9292-C8531D638853}">
-  <dimension ref="A1:B14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05B070B9-4133-4AA8-9A97-79A27B945DA7}">
+  <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13:B29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2">
+      <c r="A2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>69</v>
+      <c r="B3" s="2" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4">
-        <v>79</v>
+        <v>62</v>
+      </c>
+      <c r="B4" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>158</v>
+      <c r="A5" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <v>158</v>
+        <v>66</v>
+      </c>
+      <c r="B6" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7">
-        <v>280</v>
+        <v>67</v>
+      </c>
+      <c r="B7" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8">
-        <v>299</v>
+        <v>69</v>
+      </c>
+      <c r="B8" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9">
-        <v>796</v>
+      <c r="A9" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10">
-        <v>16348</v>
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>9</v>
+      </c>
+      <c r="B33" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>3</v>
+      </c>
+      <c r="B34" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>4</v>
+      </c>
+      <c r="B35" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>10</v>
+      </c>
+      <c r="B36" t="s">
         <v>11</v>
       </c>
-      <c r="B11">
-        <v>16348</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>12</v>
       </c>
-      <c r="B12">
-        <v>16666</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="B37" t="s">
         <v>13</v>
       </c>
-      <c r="B13">
-        <v>17000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B14">
-        <v>17777</v>
+      <c r="B38" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B092B5AC-D036-4181-B87E-BA5519C3C3E2}">
+  <dimension ref="A1:B31"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.5703125" customWidth="1"/>
+    <col min="2" max="2" width="39.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4B3B146-FFD9-4949-91F3-B88B14161C3C}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>